<commit_message>
commit salary by Hoang
</commit_message>
<xml_diff>
--- a/Huan/FB-Cleaned/[VN] Business Analytics & Decision Making Community.xlsx
+++ b/Huan/FB-Cleaned/[VN] Business Analytics & Decision Making Community.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Hoang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minh Hoang\source\repos\Teamb_Scraping_data\Huan\FB-Cleaned\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06157DC0-DBC1-4564-8932-F7E8EE7213F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0236D98-44FF-45A6-90F7-074BE26DACD3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
   <si>
     <t>User</t>
   </si>
@@ -344,6 +344,18 @@
   </si>
   <si>
     <t>0905968182</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>$700 - $1,500</t>
+  </si>
+  <si>
+    <t>9 Triệu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trên 20 triệu</t>
   </si>
 </sst>
 </file>
@@ -398,7 +410,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -411,6 +423,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -752,46 +768,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H305"/>
+  <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="116.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -802,19 +822,22 @@
         <v>31</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -825,22 +848,25 @@
         <v>37</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>92</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -853,20 +879,23 @@
       <c r="D4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" t="s">
         <v>93</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -879,20 +908,23 @@
       <c r="D5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
         <v>94</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -905,17 +937,20 @@
       <c r="D6" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -928,20 +963,23 @@
       <c r="D7" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" t="s">
         <v>95</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -954,20 +992,23 @@
       <c r="D8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" t="s">
         <v>96</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -980,17 +1021,20 @@
       <c r="D9" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1003,17 +1047,20 @@
       <c r="D10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1026,17 +1073,20 @@
       <c r="D11" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1049,20 +1099,23 @@
       <c r="D12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" t="s">
         <v>97</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1072,23 +1125,26 @@
       <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>98</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1101,17 +1157,20 @@
       <c r="D14" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1124,20 +1183,23 @@
       <c r="D15" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
         <v>99</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1150,17 +1212,20 @@
       <c r="D16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1173,20 +1238,23 @@
       <c r="D17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" t="s">
         <v>100</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1199,20 +1267,23 @@
       <c r="D18" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" t="s">
         <v>101</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1222,23 +1293,26 @@
       <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>92</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1251,17 +1325,20 @@
       <c r="D20" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1274,20 +1351,23 @@
       <c r="D21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" t="s">
         <v>95</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1300,20 +1380,23 @@
       <c r="D22" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" t="s">
         <v>102</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1326,1172 +1409,1177 @@
       <c r="D23" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E23" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>88.343138933181763</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
-      <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
-      <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
-      <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
-      <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
-      <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
-      <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
-      <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
-      <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="1"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
-      <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
-      <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
-      <c r="G86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
-      <c r="G87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
-      <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
-      <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
-      <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
-      <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
-      <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="1"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
-      <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
-      <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="1"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
-      <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="1"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
-      <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="1"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
-      <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="1"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
-      <c r="G99" s="1"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="1"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
-      <c r="G100" s="1"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="1"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
-      <c r="G101" s="1"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="1"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
-      <c r="G102" s="1"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="1"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
-      <c r="G103" s="1"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103" s="1"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
-      <c r="G104" s="1"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104" s="1"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
-      <c r="G105" s="1"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105" s="1"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
-      <c r="G106" s="1"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="1"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
-      <c r="G107" s="1"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="1"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
-      <c r="G108" s="1"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="1"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
-      <c r="G109" s="1"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="1"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
-      <c r="G110" s="1"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="1"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
-      <c r="G111" s="1"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="1"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
-      <c r="G112" s="1"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H112" s="1"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
-      <c r="G113" s="1"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H113" s="1"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
-      <c r="G114" s="1"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H114" s="1"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
-      <c r="G115" s="1"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H115" s="1"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
-      <c r="G116" s="1"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116" s="1"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
-      <c r="G117" s="1"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H117" s="1"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
-      <c r="G118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H118" s="1"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
-      <c r="G119" s="1"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H119" s="1"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
-      <c r="G120" s="1"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H120" s="1"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
-      <c r="G121" s="1"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H121" s="1"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
-      <c r="G122" s="1"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H122" s="1"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
-      <c r="G123" s="1"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H123" s="1"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
-      <c r="G124" s="1"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H124" s="1"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
-      <c r="G125" s="1"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H125" s="1"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
-      <c r="G126" s="1"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
-      <c r="G127" s="1"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H127" s="1"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
-      <c r="G128" s="1"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H128" s="1"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
-      <c r="G129" s="1"/>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H129" s="1"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
-      <c r="G130" s="1"/>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H130" s="1"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
-      <c r="G131" s="1"/>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H131" s="1"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
-      <c r="G132" s="1"/>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H132" s="1"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
-      <c r="G133" s="1"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H133" s="1"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
-      <c r="G134" s="1"/>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H134" s="1"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
-      <c r="G135" s="1"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H135" s="1"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
-      <c r="G136" s="1"/>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H136" s="1"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="C137" s="1"/>
-      <c r="G137" s="1"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D137" s="1"/>
+      <c r="H137" s="1"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
-      <c r="G138" s="1"/>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H138" s="1"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
-      <c r="G139" s="1"/>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H139" s="1"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
-      <c r="G140" s="1"/>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H140" s="1"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
-      <c r="G141" s="1"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H141" s="1"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
-      <c r="G142" s="1"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H142" s="1"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
-      <c r="G143" s="1"/>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H143" s="1"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
-      <c r="G144" s="1"/>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H144" s="1"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
-      <c r="G145" s="1"/>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H145" s="1"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
-      <c r="G146" s="1"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H146" s="1"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
-      <c r="G147" s="1"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H147" s="1"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
-      <c r="G148" s="1"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H148" s="1"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
-      <c r="G149" s="1"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H149" s="1"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
-      <c r="G150" s="1"/>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H150" s="1"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
-      <c r="G151" s="1"/>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H151" s="1"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
-      <c r="G152" s="1"/>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H152" s="1"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
-      <c r="G153" s="1"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H153" s="1"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
-      <c r="G154" s="1"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H154" s="1"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
-      <c r="G155" s="1"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H155" s="1"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
-      <c r="G156" s="1"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H156" s="1"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
-      <c r="G157" s="1"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H157" s="1"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
-      <c r="G158" s="1"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H158" s="1"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
-      <c r="G159" s="1"/>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H159" s="1"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
-      <c r="G160" s="1"/>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H160" s="1"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
-      <c r="G161" s="1"/>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H161" s="1"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
-      <c r="G162" s="1"/>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H162" s="1"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
-      <c r="G163" s="1"/>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H163" s="1"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
-      <c r="G164" s="1"/>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H164" s="1"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
-      <c r="G165" s="1"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H165" s="1"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
-      <c r="G166" s="1"/>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H166" s="1"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
-      <c r="G167" s="1"/>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H167" s="1"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
-      <c r="G168" s="1"/>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H168" s="1"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
-      <c r="G169" s="1"/>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H169" s="1"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
-      <c r="G170" s="1"/>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H170" s="1"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
-      <c r="G171" s="1"/>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H171" s="1"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
-      <c r="G172" s="1"/>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H172" s="1"/>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
-      <c r="G173" s="1"/>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H173" s="1"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
-      <c r="G174" s="1"/>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H174" s="1"/>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
-      <c r="G175" s="1"/>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H175" s="1"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
-      <c r="G176" s="1"/>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H176" s="1"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
-      <c r="G177" s="1"/>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H177" s="1"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
-      <c r="G178" s="1"/>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H178" s="1"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
-      <c r="G179" s="1"/>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H179" s="1"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
-      <c r="G180" s="1"/>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H180" s="1"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
-      <c r="G181" s="1"/>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H181" s="1"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
-      <c r="G182" s="1"/>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H182" s="1"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
-      <c r="G183" s="1"/>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H183" s="1"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
-      <c r="G184" s="1"/>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H184" s="1"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
-      <c r="G185" s="1"/>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H185" s="1"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
-      <c r="G186" s="1"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H186" s="1"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
-      <c r="G187" s="1"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H187" s="1"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
-      <c r="G188" s="1"/>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H188" s="1"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
-      <c r="G189" s="1"/>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H189" s="1"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
-      <c r="G190" s="1"/>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H190" s="1"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
-      <c r="G191" s="1"/>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H191" s="1"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
-      <c r="G192" s="1"/>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H192" s="1"/>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
-      <c r="G193" s="1"/>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H193" s="1"/>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
-      <c r="G194" s="1"/>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H194" s="1"/>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
-      <c r="G195" s="1"/>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H195" s="1"/>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
-      <c r="G196" s="1"/>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H196" s="1"/>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
-      <c r="G197" s="1"/>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H197" s="1"/>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
-      <c r="G198" s="1"/>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H198" s="1"/>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
-      <c r="G199" s="1"/>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H199" s="1"/>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
-      <c r="G200" s="1"/>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H200" s="1"/>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
-      <c r="G201" s="1"/>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H201" s="1"/>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
-      <c r="G202" s="1"/>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H202" s="1"/>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
-      <c r="G203" s="1"/>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H203" s="1"/>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
-      <c r="G204" s="1"/>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H204" s="1"/>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
-      <c r="G205" s="1"/>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H205" s="1"/>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
-      <c r="G206" s="1"/>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H206" s="1"/>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
-      <c r="G207" s="1"/>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H207" s="1"/>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
-      <c r="G208" s="1"/>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H208" s="1"/>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
-      <c r="G209" s="1"/>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H209" s="1"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
-      <c r="G210" s="1"/>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H210" s="1"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
-      <c r="G211" s="1"/>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H211" s="1"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
-      <c r="G212" s="1"/>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H212" s="1"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
-      <c r="G213" s="1"/>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H213" s="1"/>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
-      <c r="G214" s="1"/>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H214" s="1"/>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
-      <c r="G215" s="1"/>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H215" s="1"/>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
-      <c r="G216" s="1"/>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H216" s="1"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
-      <c r="G217" s="1"/>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H217" s="1"/>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
-      <c r="G218" s="1"/>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H218" s="1"/>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
-      <c r="G219" s="1"/>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H219" s="1"/>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
-      <c r="G220" s="1"/>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H220" s="1"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
-      <c r="G221" s="1"/>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H221" s="1"/>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
-      <c r="G222" s="1"/>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H222" s="1"/>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
-      <c r="G223" s="1"/>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H223" s="1"/>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
-      <c r="G224" s="1"/>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H224" s="1"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
-      <c r="G225" s="1"/>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H225" s="1"/>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
-      <c r="G226" s="1"/>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H226" s="1"/>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
-      <c r="G227" s="1"/>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H227" s="1"/>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
-      <c r="G228" s="1"/>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H228" s="1"/>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
-      <c r="G229" s="1"/>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H229" s="1"/>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
-      <c r="G230" s="1"/>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H230" s="1"/>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
-      <c r="G231" s="1"/>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H231" s="1"/>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
-      <c r="G232" s="1"/>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H232" s="1"/>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
-      <c r="G233" s="1"/>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H233" s="1"/>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
-      <c r="G234" s="1"/>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H234" s="1"/>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
-      <c r="G235" s="1"/>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H235" s="1"/>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
-      <c r="G236" s="1"/>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H236" s="1"/>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
-      <c r="G237" s="1"/>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H237" s="1"/>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
-      <c r="G238" s="1"/>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H238" s="1"/>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
-      <c r="G239" s="1"/>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H239" s="1"/>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
-      <c r="G240" s="1"/>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H240" s="1"/>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
-      <c r="G241" s="1"/>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H241" s="1"/>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
-      <c r="G242" s="1"/>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H242" s="1"/>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
-      <c r="G243" s="1"/>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H243" s="1"/>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
-      <c r="G244" s="1"/>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H244" s="1"/>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
-      <c r="G245" s="1"/>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H245" s="1"/>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
-      <c r="G246" s="1"/>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H246" s="1"/>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
-      <c r="G247" s="1"/>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H247" s="1"/>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
-      <c r="G248" s="1"/>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H248" s="1"/>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
-      <c r="G249" s="1"/>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H249" s="1"/>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
-      <c r="G250" s="1"/>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H250" s="1"/>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
-      <c r="G251" s="1"/>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H251" s="1"/>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
-      <c r="G252" s="1"/>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H252" s="1"/>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
-      <c r="G253" s="1"/>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H253" s="1"/>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
-      <c r="G254" s="1"/>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H254" s="1"/>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
-      <c r="G255" s="1"/>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H255" s="1"/>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
-      <c r="G256" s="1"/>
-    </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H256" s="1"/>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
-      <c r="G257" s="1"/>
-    </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H257" s="1"/>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
-      <c r="G258" s="1"/>
-    </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H258" s="1"/>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
-      <c r="G259" s="1"/>
-    </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H259" s="1"/>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
-      <c r="G260" s="1"/>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H260" s="1"/>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
-      <c r="G261" s="1"/>
-    </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H261" s="1"/>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="2"/>
-      <c r="G262" s="1"/>
-    </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H262" s="1"/>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="2"/>
-      <c r="G263" s="1"/>
-    </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H263" s="1"/>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
-      <c r="G264" s="1"/>
-    </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H264" s="1"/>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="2"/>
-      <c r="G265" s="1"/>
-    </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H265" s="1"/>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="2"/>
-      <c r="G266" s="1"/>
-    </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H266" s="1"/>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="2"/>
-      <c r="G267" s="1"/>
-    </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H267" s="1"/>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>
-      <c r="G268" s="1"/>
-    </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H268" s="1"/>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="2"/>
-      <c r="G269" s="1"/>
-    </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H269" s="1"/>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="2"/>
-      <c r="G270" s="1"/>
-    </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H270" s="1"/>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
-      <c r="G271" s="1"/>
-    </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H271" s="1"/>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
-      <c r="G272" s="1"/>
-    </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H272" s="1"/>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
-      <c r="G273" s="1"/>
-    </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H273" s="1"/>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
-      <c r="G274" s="1"/>
-    </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H274" s="1"/>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2"/>
-      <c r="G275" s="1"/>
-    </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H275" s="1"/>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2"/>
-      <c r="G276" s="1"/>
-    </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H276" s="1"/>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2"/>
-      <c r="G277" s="1"/>
-    </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H277" s="1"/>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2"/>
-      <c r="G278" s="1"/>
-    </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H278" s="1"/>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="2"/>
-      <c r="G279" s="1"/>
-    </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H279" s="1"/>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="2"/>
-      <c r="G280" s="1"/>
-    </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H280" s="1"/>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="2"/>
-      <c r="G281" s="1"/>
-    </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H281" s="1"/>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="2"/>
-      <c r="G282" s="1"/>
-    </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H282" s="1"/>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="2"/>
-      <c r="G283" s="1"/>
-    </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H283" s="1"/>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" s="2"/>
-      <c r="G284" s="1"/>
-    </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H284" s="1"/>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" s="2"/>
-      <c r="G285" s="1"/>
-    </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H285" s="1"/>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286" s="2"/>
-      <c r="G286" s="1"/>
-    </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H286" s="1"/>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287" s="2"/>
-      <c r="G287" s="1"/>
-    </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H287" s="1"/>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="2"/>
-      <c r="G288" s="1"/>
-    </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H288" s="1"/>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" s="2"/>
-      <c r="G289" s="1"/>
-    </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H289" s="1"/>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" s="2"/>
-      <c r="G290" s="1"/>
-    </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H290" s="1"/>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" s="2"/>
-      <c r="G291" s="1"/>
-    </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H291" s="1"/>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" s="2"/>
-      <c r="G292" s="1"/>
-    </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H292" s="1"/>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" s="2"/>
-      <c r="G293" s="1"/>
-    </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H293" s="1"/>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" s="2"/>
-      <c r="G294" s="1"/>
-    </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H294" s="1"/>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" s="2"/>
-      <c r="G295" s="1"/>
-    </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H295" s="1"/>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" s="2"/>
-      <c r="G296" s="1"/>
-    </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H296" s="1"/>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" s="2"/>
-      <c r="G297" s="1"/>
-    </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H297" s="1"/>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" s="2"/>
-      <c r="G298" s="1"/>
-    </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H298" s="1"/>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" s="2"/>
-      <c r="G299" s="1"/>
-    </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H299" s="1"/>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" s="2"/>
-      <c r="G300" s="1"/>
-    </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H300" s="1"/>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" s="2"/>
-      <c r="G301" s="1"/>
-    </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H301" s="1"/>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" s="2"/>
-      <c r="G302" s="1"/>
-    </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H302" s="1"/>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
-      <c r="D303" s="3"/>
-      <c r="F303" s="2"/>
+      <c r="D303" s="2"/>
+      <c r="E303" s="3"/>
       <c r="G303" s="2"/>
       <c r="H303" s="2"/>
-    </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I303" s="2"/>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
-      <c r="G304" s="1"/>
-    </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H304" s="1"/>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="2"/>
-      <c r="G305" s="1"/>
+      <c r="H305" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H305">
+  <sortState ref="A2:I305">
     <sortCondition ref="C2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G2" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="G22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="G6" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="G18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="G3" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="G7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="G11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="G19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="G20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="G17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="G23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="G4" r:id="rId20" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="G16" r:id="rId21" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="G21" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="H15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H2" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="H22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="H6" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="H18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="H3" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="H7" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="H11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="H20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="H17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="H23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="H4" r:id="rId20" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="H16" r:id="rId21" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="H21" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>

</xml_diff>